<commit_message>
change data/annotations => data/csv_files
</commit_message>
<xml_diff>
--- a/outputs/tables/kappa.xlsx
+++ b/outputs/tables/kappa.xlsx
@@ -1,37 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>1dAVb</t>
+  </si>
+  <si>
+    <t>RBBB</t>
+  </si>
+  <si>
+    <t>LBBB</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>DNN vs cardio.</t>
+  </si>
+  <si>
+    <t>DNN vs emerg.</t>
+  </si>
+  <si>
+    <t>DNN vs stud.</t>
+  </si>
+  <si>
+    <t>cardio. vs emerg.</t>
+  </si>
+  <si>
+    <t>cardio. vs stud.</t>
+  </si>
+  <si>
+    <t>emerg. vs stud.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +90,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -353,202 +406,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>1dAVb</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>RBBB</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>LBBB</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SB</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>AF</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ST</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>DNN vs cardio.</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>0.656</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>0.917</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>0.945</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0.83</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>0.78</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0.864</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>DNN vs emerg.</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
         <v>0.6840000000000001</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>0.792</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>0.909</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0.796</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>0.595</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>0.93</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>DNN vs stud.</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
         <v>0.642</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0.928</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>0.912</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0.76</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>0.574</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>0.855</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>cardio. vs emerg.</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
         <v>0.656</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>0.824</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>0.923</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>0.912</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>0.515</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>0.847</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>cardio. vs stud.</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
         <v>0.612</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>0.871</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>0.889</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>0.88</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>0.7</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>0.792</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>emerg. vs stud.</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
         <v>0.615</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>0.799</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>0.852</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>0.907</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>0.508</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>0.897</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>